<commit_message>
Mac template and DEP/PIP demotion
</commit_message>
<xml_diff>
--- a/site/application/backend/app-forms/View/Layouts/mac-template.xlsx
+++ b/site/application/backend/app-forms/View/Layouts/mac-template.xlsx
@@ -14,13 +14,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
+    <t>&lt;Department&gt;</t>
+  </si>
+  <si>
     <t>2015 STATUS as at &lt;DATE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;YEAR&gt;</t>
+  </si>
+  <si>
+    <t>Budget</t>
   </si>
   <si>
     <t>&lt;YEAR&gt; Progess to Target</t>
   </si>
   <si>
+    <t>Unrestricted</t>
+  </si>
+  <si>
     <t xml:space="preserve"> &lt;YEAR&gt; Budget Targets</t>
+  </si>
+  <si>
+    <t>Confirmed Funding</t>
   </si>
   <si>
     <t>Progress Status to Targets Against Budget 
@@ -30,14 +45,32 @@
     <t>Pipeline  (all unconfirmed)</t>
   </si>
   <si>
-    <t>Comparison Figures as at &lt;DATE&gt;
+    <t>Country/Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparison Figures as at &lt;DATE&gt;
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project </t>
+  </si>
+  <si>
+    <t>Fund Code</t>
+  </si>
+  <si>
+    <t>Donor</t>
   </si>
   <si>
     <t xml:space="preserve">PROGRAMME </t>
   </si>
   <si>
+    <t>Dates</t>
+  </si>
+  <si>
     <t xml:space="preserve">Budget </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Value    </t>
   </si>
   <si>
     <t>Unrestricted 
@@ -45,6 +78,9 @@
   </si>
   <si>
     <t>Confirmed</t>
+  </si>
+  <si>
+    <t>% MF Achieved</t>
   </si>
   <si>
     <t>Confirmed &amp; Highly Likely (CF/HL)</t>
@@ -59,46 +95,10 @@
     <t>Low to Medium</t>
   </si>
   <si>
-    <t>Budget</t>
-  </si>
-  <si>
     <t>Value CF&amp;HL</t>
   </si>
   <si>
     <t>CF/HL</t>
-  </si>
-  <si>
-    <t>&lt;Department&gt;</t>
-  </si>
-  <si>
-    <t>&lt;YEAR&gt;</t>
-  </si>
-  <si>
-    <t>Unrestricted</t>
-  </si>
-  <si>
-    <t>Confirmed Funding</t>
-  </si>
-  <si>
-    <t>Country/Area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project </t>
-  </si>
-  <si>
-    <t>Fund Code</t>
-  </si>
-  <si>
-    <t>Donor</t>
-  </si>
-  <si>
-    <t>Dates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Value    </t>
-  </si>
-  <si>
-    <t>% MF Achieved</t>
   </si>
   <si>
     <t>TOTAL CONFIRMED AGAINST BUDGET</t>
@@ -143,11 +143,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@"/>
-    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0;\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="167" formatCode="d/m/yy"/>
-    <numFmt numFmtId="168" formatCode="dd/MM/yyyy"/>
-    <numFmt numFmtId="169" formatCode="[$£]#,##0"/>
+    <numFmt numFmtId="165" formatCode="d/m/yy"/>
+    <numFmt numFmtId="166" formatCode="dd/MM/yyyy"/>
+    <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="168" formatCode="[$£]#,##0"/>
+    <numFmt numFmtId="169" formatCode="&quot;£&quot;#,##0;\-&quot;£&quot;#,##0"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -156,12 +156,27 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="14.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial Narrow"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color rgb="FF205867"/>
       <name val="Trebuchet MS"/>
     </font>
     <font/>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF632423"/>
+      <name val="'Arial Narrow'"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF632423"/>
+      <name val="Arial Narrow"/>
+    </font>
     <font>
       <b/>
       <sz val="10.0"/>
@@ -178,10 +193,21 @@
       <name val="Trebuchet MS"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial Narrow"/>
+    </font>
+    <font>
       <b/>
       <sz val="12.0"/>
       <color rgb="FF205867"/>
       <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.0"/>
+      <color rgb="FF632423"/>
+      <name val="Arial Narrow"/>
     </font>
     <font>
       <b/>
@@ -203,59 +229,13 @@
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
-      <name val="Trebuchet MS"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11.0"/>
-      <name val="Trebuchet MS"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11.0"/>
-      <color rgb="FF1F497D"/>
-      <name val="Trebuchet MS"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF1F497D"/>
-      <name val="Trebuchet MS"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <name val="Trebuchet MS"/>
-    </font>
-    <font>
-      <sz val="14.0"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial Narrow"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color rgb="FF632423"/>
-      <name val="'Arial Narrow'"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color rgb="FF632423"/>
-      <name val="Arial Narrow"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="8.0"/>
       <name val="Arial Narrow"/>
     </font>
     <font>
       <b/>
-      <sz val="9.0"/>
-      <color rgb="FF632423"/>
-      <name val="Arial Narrow"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8.0"/>
-      <name val="Arial Narrow"/>
+      <sz val="10.0"/>
+      <name val="Trebuchet MS"/>
     </font>
     <font>
       <b/>
@@ -274,9 +254,29 @@
     </font>
     <font>
       <b/>
+      <sz val="11.0"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF1F497D"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF1F497D"/>
+      <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Trebuchet MS"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -315,8 +315,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEEECE1"/>
-        <bgColor rgb="FFEEECE1"/>
+        <fgColor rgb="FF953734"/>
+        <bgColor rgb="FF953734"/>
       </patternFill>
     </fill>
     <fill>
@@ -327,20 +327,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEEECE1"/>
+        <bgColor rgb="FFEEECE1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF366092"/>
         <bgColor rgb="FF366092"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF953734"/>
-        <bgColor rgb="FF953734"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6E3BC"/>
+        <bgColor rgb="FFD6E3BC"/>
       </patternFill>
     </fill>
     <fill>
@@ -361,24 +373,22 @@
         <bgColor rgb="FFDDD9C3"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD6E3BC"/>
-        <bgColor rgb="FFD6E3BC"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
     </border>
     <border>
@@ -399,15 +409,11 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -430,22 +436,16 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color rgb="FF000000"/>
-      </left>
-      <right/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <bottom style="thin">
         <color rgb="FF000000"/>
-      </top>
-      <bottom/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -501,217 +501,217 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="11" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="5" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="5" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="2" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="6" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="15" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="7" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="16" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="6" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="11" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="7" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="8" fontId="19" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="9" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="8" fontId="19" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="10" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="8" fontId="19" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="10" fontId="21" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="8" fontId="19" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="8" fontId="19" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="10" fontId="20" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="8" fontId="11" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="8" fontId="11" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="9" fontId="11" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="9" fontId="11" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="13" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="14" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="14" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="14" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="14" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="14" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="17" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="17" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="17" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="10" fontId="20" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="10" fontId="20" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="22" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="11" fontId="20" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="11" fontId="20" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="23" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="24" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="24" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="24" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="4" fontId="24" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="22" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="24" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="19" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="19" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="26" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="20" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="26" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="26" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="10" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="11" fontId="23" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="11" fontId="23" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="27" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="19" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="28" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="19" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="19" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="11" fontId="23" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="11" fontId="23" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="11" fontId="23" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="24" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="24" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="26" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="26" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="26" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="19" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="19" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="19" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="19" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="27" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="23" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="28" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="23" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="23" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -723,11 +723,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -738,378 +738,380 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="27" width="13.25"/>
+    <col customWidth="1" min="1" max="3" width="13.25"/>
+    <col customWidth="1" min="4" max="4" width="19.88"/>
+    <col customWidth="1" min="5" max="27" width="13.25"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" ht="34.5" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>2</v>
+      <c r="A2" s="13" t="s">
+        <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" ht="30.75" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="7" t="s">
-        <v>4</v>
+      <c r="L3" s="33" t="s">
+        <v>26</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="8" t="s">
-        <v>5</v>
+      <c r="M3" s="33" t="s">
+        <v>27</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="5"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="5"/>
+      <c r="N3" s="11"/>
     </row>
     <row r="4">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="5"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="5"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="11"/>
     </row>
     <row r="6">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="5"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="5"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="8">
-      <c r="A8" s="32"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="5"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="32"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="5"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="5"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="11"/>
     </row>
     <row r="12">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
     </row>
     <row r="16">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
     </row>
     <row r="17">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
     </row>
     <row r="18">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
     </row>
     <row r="21">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1143,147 +1145,147 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="33" t="s">
-        <v>17</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="12"/>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" ht="32.25" customHeight="1">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="38"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="39"/>
-      <c r="F2" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="38"/>
-    </row>
-    <row r="3" ht="32.25" customHeight="1">
-      <c r="A3" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="41" t="s">
+      <c r="H4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="41" t="s">
-        <v>22</v>
+      <c r="I4" s="27" t="s">
+        <v>2</v>
       </c>
-      <c r="C4" s="41" t="s">
-        <v>23</v>
+      <c r="J4" s="27" t="s">
+        <v>2</v>
       </c>
-      <c r="D4" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="46" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
     </row>
     <row r="6">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
     </row>
     <row r="7">
-      <c r="A7" s="56"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
     </row>
     <row r="8" ht="29.25" customHeight="1">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9">
       <c r="A9" s="61" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B9" s="61" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C9" s="61" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="61" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E9" s="62" t="s">
         <v>31</v>
@@ -1297,18 +1299,18 @@
       <c r="H9" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="46" t="s">
-        <v>18</v>
+      <c r="I9" s="27" t="s">
+        <v>2</v>
       </c>
-      <c r="J9" s="46" t="s">
-        <v>18</v>
+      <c r="J9" s="27" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="65"/>
       <c r="F10" s="66"/>
       <c r="G10" s="67"/>
@@ -1320,13 +1322,13 @@
       <c r="A11" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="70"/>
       <c r="J11" s="71"/>
     </row>
@@ -1334,13 +1336,13 @@
       <c r="A12" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="72"/>
       <c r="J12" s="72"/>
     </row>
@@ -1348,25 +1350,25 @@
       <c r="A13" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="54"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="43"/>
       <c r="I13" s="74"/>
       <c r="J13" s="74"/>
     </row>
     <row r="14">
-      <c r="A14" s="56"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="58"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="55"/>
       <c r="I14" s="75"/>
       <c r="J14" s="75"/>
     </row>
@@ -1377,14 +1379,14 @@
       <c r="B15" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16">
       <c r="B16" s="78"/>

</xml_diff>